<commit_message>
Added Final Exam to Timeline
</commit_message>
<xml_diff>
--- a/CMP168_TimeLine.xlsx
+++ b/CMP168_TimeLine.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="57">
   <si>
     <t>Week</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Ch15 - Recursion &amp; unveil project 2</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
   </si>
 </sst>
 </file>
@@ -795,10 +798,10 @@
   <dimension ref="A1:Y1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2360,8 +2363,12 @@
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" s="12"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="14"/>
+      <c r="G66" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="I66" s="12"/>
       <c r="J66" s="15"/>
       <c r="K66" s="12"/>
@@ -2379,8 +2386,12 @@
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
       <c r="F67" s="20"/>
-      <c r="G67" s="63"/>
-      <c r="H67" s="63"/>
+      <c r="G67" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="H67" s="63" t="s">
+        <v>56</v>
+      </c>
       <c r="I67" s="20"/>
       <c r="J67" s="24"/>
       <c r="K67" s="20"/>
@@ -2398,8 +2409,12 @@
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="12"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
+      <c r="G68" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="I68" s="12"/>
       <c r="J68" s="15"/>
       <c r="K68" s="12"/>
@@ -2417,8 +2432,12 @@
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
       <c r="F69" s="20"/>
-      <c r="G69" s="63"/>
-      <c r="H69" s="63"/>
+      <c r="G69" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="H69" s="63" t="s">
+        <v>56</v>
+      </c>
       <c r="I69" s="20"/>
       <c r="J69" s="24"/>
       <c r="K69" s="20"/>

</xml_diff>